<commit_message>
Changes in sonarqube config 6
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/secure-reports/monthreports/Attendance_from_2025-02_to_2025-03.xlsx
+++ b/backend/slack-hrbp/secure-reports/monthreports/Attendance_from_2025-02_to_2025-03.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="91">
   <si>
     <t>User Name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Saathwik</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Ram</t>
   </si>
   <si>
     <t>Shreya</t>
@@ -324,7 +330,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AE16"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1850,6 +1856,196 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="L17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="O17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Q17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="S17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="U17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="V17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="W17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="X17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Y17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Z17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AA17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AB17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AC17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AD17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AE17" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="O18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Q18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="S18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="U18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="V18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="W18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="X18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Y18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Z18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AA18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AB18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AC18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AD18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AE18" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1857,7 +2053,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1874,97 +2070,97 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s" s="0">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M1" t="s" s="0">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s" s="0">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O1" t="s" s="0">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P1" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q1" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R1" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="S1" t="s" s="0">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="T1" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="U1" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="V1" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="W1" t="s" s="0">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="X1" t="s" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Y1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AA1" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AB1" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AC1" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AD1" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AE1" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AF1" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AG1" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AH1" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
@@ -2183,7 +2379,7 @@
         <v>32</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>33</v>
@@ -2243,13 +2439,13 @@
         <v>33</v>
       </c>
       <c r="W4" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="X4" t="s" s="0">
         <v>33</v>
       </c>
       <c r="Y4" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Z4" t="s" s="0">
         <v>33</v>
@@ -2287,7 +2483,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>33</v>
@@ -2332,7 +2528,7 @@
         <v>33</v>
       </c>
       <c r="R5" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S5" t="s" s="0">
         <v>33</v>
@@ -2388,13 +2584,13 @@
         <v>39</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>33</v>
@@ -2492,7 +2688,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>32</v>
@@ -2570,7 +2766,7 @@
         <v>33</v>
       </c>
       <c r="AB7" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AC7" t="s" s="0">
         <v>36</v>
@@ -2579,7 +2775,7 @@
         <v>33</v>
       </c>
       <c r="AE7" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AF7" t="s" s="0">
         <v>33</v>
@@ -2703,7 +2899,7 @@
         <v>32</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>33</v>
@@ -2748,7 +2944,7 @@
         <v>33</v>
       </c>
       <c r="R9" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S9" t="s" s="0">
         <v>33</v>
@@ -2804,10 +3000,10 @@
         <v>43</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>33</v>
@@ -2861,16 +3057,16 @@
         <v>36</v>
       </c>
       <c r="U10" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="V10" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="W10" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="X10" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Y10" t="s" s="0">
         <v>36</v>
@@ -3015,7 +3211,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s" s="0">
         <v>33</v>
@@ -3051,7 +3247,7 @@
         <v>33</v>
       </c>
       <c r="O12" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P12" t="s" s="0">
         <v>33</v>
@@ -3324,7 +3520,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>32</v>
@@ -3405,7 +3601,7 @@
         <v>36</v>
       </c>
       <c r="AC15" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AD15" t="s" s="0">
         <v>36</v>
@@ -3524,6 +3720,214 @@
         <v>33</v>
       </c>
       <c r="AH16" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="L17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="O17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Q17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="S17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="U17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="V17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="W17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="X17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Y17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Z17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AA17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AB17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AC17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AD17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AE17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AF17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AG17" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AH17" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="O18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Q18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="S18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="U18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="V18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="W18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="X18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Y18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="Z18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AA18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AB18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AC18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AD18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AE18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AF18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AG18" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AH18" t="s" s="0">
         <v>33</v>
       </c>
     </row>

</xml_diff>